<commit_message>
Major type group implementation
</commit_message>
<xml_diff>
--- a/docs/Fieldwork/People list.xlsx
+++ b/docs/Fieldwork/People list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amarok/src/natur-i-norge/docs/Fieldwork/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8837033-5A31-E646-8834-F2FE852A6A2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C58802F-9D2D-6042-9F93-6D14C2074845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{4624BE88-9AAE-9C4E-B444-E4CB5E687DFF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4624BE88-9AAE-9C4E-B444-E4CB5E687DFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -695,7 +695,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="237" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>

</xml_diff>